<commit_message>
Initial object model setup
</commit_message>
<xml_diff>
--- a/c_resources/port_royal_simple_model.xlsx
+++ b/c_resources/port_royal_simple_model.xlsx
@@ -8,12 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\JPr\code\port_royal\c_resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D448B4E9-2D5C-4A6F-96E2-35225ED59D9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B6729D3-49A2-496E-AA2F-B66577CB0EE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="9600" yWindow="0" windowWidth="9600" windowHeight="10200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="abstract_objects" sheetId="1" r:id="rId1"/>
+    <sheet name="concrete_objects" sheetId="2" r:id="rId2"/>
+    <sheet name="enums" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,16 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="15">
-  <si>
-    <t>super_classes</t>
-  </si>
-  <si>
-    <t>classes</t>
-  </si>
-  <si>
-    <t>compositions</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="56">
   <si>
     <t>GameTypes</t>
   </si>
@@ -70,13 +63,145 @@
   </si>
   <si>
     <t>PortRoyalPlayerBoards</t>
+  </si>
+  <si>
+    <t>implemented</t>
+  </si>
+  <si>
+    <t>PortRoyalDices</t>
+  </si>
+  <si>
+    <t>PortRoyalColorDices</t>
+  </si>
+  <si>
+    <t>PortRoyalLetterDices</t>
+  </si>
+  <si>
+    <t>class_names</t>
+  </si>
+  <si>
+    <t>super_class_names</t>
+  </si>
+  <si>
+    <t>composition_names</t>
+  </si>
+  <si>
+    <t>attribute_names</t>
+  </si>
+  <si>
+    <t>attribute_values</t>
+  </si>
+  <si>
+    <t>PortRoyalPlayAreaPieces</t>
+  </si>
+  <si>
+    <t>PortRoyalSteeringWheels</t>
+  </si>
+  <si>
+    <t>PortRoyalShips</t>
+  </si>
+  <si>
+    <t>SteeringWheelsRed</t>
+  </si>
+  <si>
+    <t>SteeringWheelsBlue</t>
+  </si>
+  <si>
+    <t>SteeringWheelsYellow</t>
+  </si>
+  <si>
+    <t>SteeringWheelsGreen</t>
+  </si>
+  <si>
+    <t>SteeringWheelsOrange</t>
+  </si>
+  <si>
+    <t>ShipsRed</t>
+  </si>
+  <si>
+    <t>ShipsBlue</t>
+  </si>
+  <si>
+    <t>ShipsYellow</t>
+  </si>
+  <si>
+    <t>ShipsGreen</t>
+  </si>
+  <si>
+    <t>ShipsOrange</t>
+  </si>
+  <si>
+    <t>ShipsBlack</t>
+  </si>
+  <si>
+    <t>PlayerBoardIslands</t>
+  </si>
+  <si>
+    <t>GameUniverseGamePieces</t>
+  </si>
+  <si>
+    <t>PortRoyalPlayerBoardPieces</t>
+  </si>
+  <si>
+    <t>saber_value</t>
+  </si>
+  <si>
+    <t>per_roll_limit</t>
+  </si>
+  <si>
+    <t>repeats the roll</t>
+  </si>
+  <si>
+    <t>temporarily adds sabers</t>
+  </si>
+  <si>
+    <t>used_in_phase</t>
+  </si>
+  <si>
+    <t>if there are at least 4 wheels/steering wheels of any composition on the board before your choice, you may tick 3 squares of your choice on your game board</t>
+  </si>
+  <si>
+    <t>function_notes</t>
+  </si>
+  <si>
+    <t>doubles the points of yellow ships</t>
+  </si>
+  <si>
+    <t>Sailor</t>
+  </si>
+  <si>
+    <t>Pirate</t>
+  </si>
+  <si>
+    <t>Vendor</t>
+  </si>
+  <si>
+    <t>Wholesaler</t>
+  </si>
+  <si>
+    <t>Prankster</t>
+  </si>
+  <si>
+    <t>Vice Admiral</t>
+  </si>
+  <si>
+    <t>Admiral</t>
+  </si>
+  <si>
+    <t>Senorita</t>
+  </si>
+  <si>
+    <t>Passenger</t>
+  </si>
+  <si>
+    <t>PlayerBoardIslandPersons</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -84,16 +209,29 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -101,14 +239,32 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Check Cell" xfId="1" builtinId="23"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -387,120 +543,520 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:D27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="22.59765625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.53125" customWidth="1"/>
+    <col min="1" max="1" width="22.53125" customWidth="1"/>
+    <col min="2" max="2" width="23" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="33.86328125" customWidth="1"/>
+    <col min="4" max="4" width="11.73046875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A1" t="s">
+    <row r="1" spans="1:4" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="14.65" thickTop="1" x14ac:dyDescent="0.45">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A3" t="s">
         <v>1</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B3" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A2" t="s">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
         <v>5</v>
       </c>
-      <c r="B2" t="s">
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A8" t="s">
+        <v>3</v>
+      </c>
+      <c r="B8" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A3" t="s">
+      <c r="C8" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A11" t="s">
         <v>3</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B11" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A12" t="s">
+        <v>9</v>
+      </c>
+      <c r="B12" t="s">
+        <v>8</v>
+      </c>
+      <c r="C12" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A14" t="s">
+        <v>3</v>
+      </c>
+      <c r="B14" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A15" t="s">
+        <v>10</v>
+      </c>
+      <c r="B15" t="s">
+        <v>11</v>
+      </c>
+      <c r="C15" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A18" t="s">
+        <v>3</v>
+      </c>
+      <c r="B18" t="s">
+        <v>36</v>
+      </c>
+      <c r="C18" t="s">
         <v>4</v>
       </c>
-      <c r="C3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" t="s">
-        <v>6</v>
-      </c>
-      <c r="C6" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7" t="s">
-        <v>9</v>
-      </c>
-      <c r="C7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A9" t="s">
-        <v>12</v>
-      </c>
-      <c r="B9" t="s">
-        <v>6</v>
-      </c>
-      <c r="C9" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A10" t="s">
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A19" t="s">
+        <v>36</v>
+      </c>
+      <c r="B19" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A21" t="s">
+        <v>21</v>
+      </c>
+      <c r="B21" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A22" t="s">
+        <v>21</v>
+      </c>
+      <c r="B22" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A23" t="s">
+        <v>21</v>
+      </c>
+      <c r="B23" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A25" t="s">
+        <v>36</v>
+      </c>
+      <c r="B25" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A26" t="s">
+        <v>37</v>
+      </c>
+      <c r="B26" t="s">
+        <v>35</v>
+      </c>
+      <c r="C26" t="s">
         <v>11</v>
       </c>
-      <c r="B10" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A12" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A13" t="s">
-        <v>14</v>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A27" t="s">
+        <v>37</v>
+      </c>
+      <c r="B27" t="s">
+        <v>55</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF752583-041F-4833-A701-CAEDADD91A04}">
+  <dimension ref="A1:E30"/>
+  <sheetViews>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="20.796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.86328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.86328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.59765625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="14.65" thickTop="1" x14ac:dyDescent="0.45">
+      <c r="A2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C6" t="s">
+        <v>42</v>
+      </c>
+      <c r="D6">
+        <v>2</v>
+      </c>
+      <c r="E6" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A7" t="s">
+        <v>22</v>
+      </c>
+      <c r="B7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C7" t="s">
+        <v>42</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8" t="s">
+        <v>25</v>
+      </c>
+      <c r="C8" t="s">
+        <v>39</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+      <c r="E8" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A9" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9" t="s">
+        <v>26</v>
+      </c>
+      <c r="C9" t="s">
+        <v>42</v>
+      </c>
+      <c r="D9">
+        <v>2</v>
+      </c>
+      <c r="E9" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A10" t="s">
+        <v>22</v>
+      </c>
+      <c r="B10" t="s">
+        <v>27</v>
+      </c>
+      <c r="C10" t="s">
+        <v>42</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A11" t="s">
+        <v>22</v>
+      </c>
+      <c r="B11" t="s">
+        <v>28</v>
+      </c>
+      <c r="C11" t="s">
+        <v>42</v>
+      </c>
+      <c r="D11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A12" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12" t="s">
+        <v>28</v>
+      </c>
+      <c r="C12" t="s">
+        <v>38</v>
+      </c>
+      <c r="D12">
+        <v>2</v>
+      </c>
+      <c r="E12" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A13" t="s">
+        <v>22</v>
+      </c>
+      <c r="B13" t="s">
+        <v>28</v>
+      </c>
+      <c r="C13" t="s">
+        <v>39</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+      <c r="E13" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A15" t="s">
+        <v>23</v>
+      </c>
+      <c r="B15" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A16" t="s">
+        <v>23</v>
+      </c>
+      <c r="B16" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A17" t="s">
+        <v>23</v>
+      </c>
+      <c r="B17" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A18" t="s">
+        <v>23</v>
+      </c>
+      <c r="B18" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A19" t="s">
+        <v>23</v>
+      </c>
+      <c r="B19" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A20" t="s">
+        <v>23</v>
+      </c>
+      <c r="B20" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A22" t="s">
+        <v>55</v>
+      </c>
+      <c r="B22" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A23" t="s">
+        <v>55</v>
+      </c>
+      <c r="B23" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A24" t="s">
+        <v>55</v>
+      </c>
+      <c r="B24" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A25" t="s">
+        <v>55</v>
+      </c>
+      <c r="B25" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A26" t="s">
+        <v>55</v>
+      </c>
+      <c r="B26" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A27" t="s">
+        <v>55</v>
+      </c>
+      <c r="B27" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A28" t="s">
+        <v>55</v>
+      </c>
+      <c r="B28" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A29" t="s">
+        <v>55</v>
+      </c>
+      <c r="B29" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A30" t="s">
+        <v>55</v>
+      </c>
+      <c r="B30" t="s">
+        <v>54</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B61C808-932F-4D58-A0FC-A4BFD7110AE8}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>